<commit_message>
Adding all changes to Data0 as on 04/05/2019
</commit_message>
<xml_diff>
--- a/IT Returns/FORMAT/Flaps.xlsx
+++ b/IT Returns/FORMAT/Flaps.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VISHAL\Desktop\Data0\IT Returns\FORMAT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935" firstSheet="6" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935" firstSheet="9" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="AY 04-05" sheetId="15" r:id="rId1"/>
@@ -21,6 +26,8 @@
     <sheet name="AY 15-16" sheetId="7" r:id="rId12"/>
     <sheet name="AY 16-17" sheetId="8" r:id="rId13"/>
     <sheet name="AY 17-18" sheetId="16" r:id="rId14"/>
+    <sheet name="AY 18-19" sheetId="17" r:id="rId15"/>
+    <sheet name="AY 18-19 (2)" sheetId="18" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'AY 04-05'!$A$1:$N$16</definedName>
@@ -37,13 +44,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="11">'AY 15-16'!$A$1:$N$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">'AY 16-17'!$A$1:$N$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="13">'AY 17-18'!$A$1:$N$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="14">'AY 18-19'!$A$1:$N$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="15">'AY 18-19 (2)'!$A$1:$N$16</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>A.Y. 2011-12</t>
   </si>
@@ -130,13 +139,25 @@
   </si>
   <si>
     <t>F.Y. 2016-17</t>
+  </si>
+  <si>
+    <t>A.Y. 2018-19</t>
+  </si>
+  <si>
+    <t>F.Y. 2017-18</t>
+  </si>
+  <si>
+    <t>F.Y. 2018-19</t>
+  </si>
+  <si>
+    <t>GST Challans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,9 +301,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,6 +336,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -489,29 +512,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="4:17" ht="30" customHeight="1"/>
-    <row r="3" spans="4:17" ht="30" customHeight="1"/>
-    <row r="4" spans="4:17" ht="30" customHeight="1"/>
-    <row r="5" spans="4:17" ht="30" customHeight="1">
+    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="30" customHeight="1">
+    <row r="6" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
@@ -524,7 +547,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:17" ht="30" customHeight="1">
+    <row r="7" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -535,7 +558,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="4:17" ht="30" customHeight="1">
+    <row r="8" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -547,7 +570,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:17" ht="30" customHeight="1">
+    <row r="9" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
@@ -560,7 +583,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="4:17" ht="30" customHeight="1">
+    <row r="10" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -571,7 +594,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:17" ht="30" customHeight="1">
+    <row r="11" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -582,11 +605,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:17" ht="30" customHeight="1"/>
-    <row r="13" spans="4:17" ht="30" customHeight="1"/>
-    <row r="14" spans="4:17" ht="30" customHeight="1"/>
-    <row r="15" spans="4:17" ht="30" customHeight="1"/>
-    <row r="16" spans="4:17" ht="30" customHeight="1"/>
+    <row r="12" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -598,25 +621,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="6:14" ht="30" customHeight="1"/>
-    <row r="3" spans="6:14" ht="30" customHeight="1"/>
-    <row r="4" spans="6:14" ht="30" customHeight="1"/>
-    <row r="5" spans="6:14" ht="30" customHeight="1"/>
-    <row r="6" spans="6:14" ht="30" customHeight="1">
+    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
@@ -629,7 +652,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="6:14" ht="30" customHeight="1">
+    <row r="7" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -640,7 +663,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="6:14" ht="30" customHeight="1">
+    <row r="8" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -651,7 +674,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="6:14" ht="30" customHeight="1">
+    <row r="9" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>1</v>
       </c>
@@ -664,7 +687,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="6:14" ht="30" customHeight="1">
+    <row r="10" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -675,7 +698,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="6:14" ht="30" customHeight="1">
+    <row r="11" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -686,11 +709,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="6:14" ht="30" customHeight="1"/>
-    <row r="13" spans="6:14" ht="30" customHeight="1"/>
-    <row r="14" spans="6:14" ht="30" customHeight="1"/>
-    <row r="15" spans="6:14" ht="30" customHeight="1"/>
-    <row r="16" spans="6:14" ht="30" customHeight="1"/>
+    <row r="12" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -702,25 +725,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="6:14" ht="30" customHeight="1"/>
-    <row r="3" spans="6:14" ht="30" customHeight="1"/>
-    <row r="4" spans="6:14" ht="30" customHeight="1"/>
-    <row r="5" spans="6:14" ht="30" customHeight="1"/>
-    <row r="6" spans="6:14" ht="30" customHeight="1">
+    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>6</v>
       </c>
@@ -733,7 +756,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="6:14" ht="30" customHeight="1">
+    <row r="7" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -744,7 +767,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="6:14" ht="30" customHeight="1">
+    <row r="8" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -755,7 +778,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="6:14" ht="30" customHeight="1">
+    <row r="9" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>3</v>
       </c>
@@ -768,7 +791,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="6:14" ht="30" customHeight="1">
+    <row r="10" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -779,7 +802,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="6:14" ht="30" customHeight="1">
+    <row r="11" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -790,11 +813,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="6:14" ht="30" customHeight="1"/>
-    <row r="13" spans="6:14" ht="30" customHeight="1"/>
-    <row r="14" spans="6:14" ht="30" customHeight="1"/>
-    <row r="15" spans="6:14" ht="30" customHeight="1"/>
-    <row r="16" spans="6:14" ht="30" customHeight="1"/>
+    <row r="12" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -806,25 +829,25 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="6:14" ht="30" customHeight="1"/>
-    <row r="3" spans="6:14" ht="30" customHeight="1"/>
-    <row r="4" spans="6:14" ht="30" customHeight="1"/>
-    <row r="5" spans="6:14" ht="30" customHeight="1"/>
-    <row r="6" spans="6:14" ht="30" customHeight="1">
+    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>8</v>
       </c>
@@ -837,7 +860,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="6:14" ht="30" customHeight="1">
+    <row r="7" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -848,7 +871,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="6:14" ht="30" customHeight="1">
+    <row r="8" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -859,7 +882,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="6:14" ht="30" customHeight="1">
+    <row r="9" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>5</v>
       </c>
@@ -872,7 +895,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="6:14" ht="30" customHeight="1">
+    <row r="10" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -883,7 +906,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="6:14" ht="30" customHeight="1">
+    <row r="11" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -894,11 +917,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="6:14" ht="30" customHeight="1"/>
-    <row r="13" spans="6:14" ht="30" customHeight="1"/>
-    <row r="14" spans="6:14" ht="30" customHeight="1"/>
-    <row r="15" spans="6:14" ht="30" customHeight="1"/>
-    <row r="16" spans="6:14" ht="30" customHeight="1"/>
+    <row r="12" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -910,25 +933,25 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="6:14" ht="30" customHeight="1"/>
-    <row r="3" spans="6:14" ht="30" customHeight="1"/>
-    <row r="4" spans="6:14" ht="30" customHeight="1"/>
-    <row r="5" spans="6:14" ht="30" customHeight="1"/>
-    <row r="6" spans="6:14" ht="30" customHeight="1">
+    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
@@ -941,7 +964,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="6:14" ht="30" customHeight="1">
+    <row r="7" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -952,7 +975,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="6:14" ht="30" customHeight="1">
+    <row r="8" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -963,7 +986,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="6:14" ht="30" customHeight="1">
+    <row r="9" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>7</v>
       </c>
@@ -976,7 +999,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="6:14" ht="30" customHeight="1">
+    <row r="10" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -987,7 +1010,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="6:14" ht="30" customHeight="1">
+    <row r="11" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -998,11 +1021,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="6:14" ht="30" customHeight="1"/>
-    <row r="13" spans="6:14" ht="30" customHeight="1"/>
-    <row r="14" spans="6:14" ht="30" customHeight="1"/>
-    <row r="15" spans="6:14" ht="30" customHeight="1"/>
-    <row r="16" spans="6:14" ht="30" customHeight="1"/>
+    <row r="12" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1014,14 +1037,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="4" width="9.140625" style="1"/>
@@ -1031,12 +1054,12 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="6:14" ht="30" customHeight="1"/>
-    <row r="3" spans="6:14" ht="30" customHeight="1"/>
-    <row r="4" spans="6:14" ht="30" customHeight="1"/>
-    <row r="5" spans="6:14" ht="30" customHeight="1"/>
-    <row r="6" spans="6:14" ht="30" customHeight="1">
+    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
@@ -1049,7 +1072,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="6:14" ht="30" customHeight="1">
+    <row r="7" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1060,7 +1083,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="6:14" ht="30" customHeight="1">
+    <row r="8" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1071,7 +1094,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="6:14" ht="30" customHeight="1">
+    <row r="9" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1084,7 +1107,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="6:14" ht="30" customHeight="1">
+    <row r="10" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1095,7 +1118,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="6:14" ht="30" customHeight="1">
+    <row r="11" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1106,11 +1129,227 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="6:14" ht="30" customHeight="1"/>
-    <row r="13" spans="6:14" ht="30" customHeight="1"/>
-    <row r="14" spans="6:14" ht="30" customHeight="1"/>
-    <row r="15" spans="6:14" ht="30" customHeight="1"/>
-    <row r="16" spans="6:14" ht="30" customHeight="1"/>
+    <row r="12" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F6:M8"/>
+    <mergeCell ref="F9:M11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="7" style="1" customWidth="1"/>
+    <col min="6" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F6:M8"/>
+    <mergeCell ref="F9:M11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="7" style="1" customWidth="1"/>
+    <col min="6" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1122,29 +1361,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="4:17" ht="30" customHeight="1"/>
-    <row r="3" spans="4:17" ht="30" customHeight="1"/>
-    <row r="4" spans="4:17" ht="30" customHeight="1"/>
-    <row r="5" spans="4:17" ht="30" customHeight="1">
+    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="30" customHeight="1">
+    <row r="6" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1396,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:17" ht="30" customHeight="1">
+    <row r="7" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1168,7 +1407,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="4:17" ht="30" customHeight="1">
+    <row r="8" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1180,7 +1419,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:17" ht="30" customHeight="1">
+    <row r="9" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1193,7 +1432,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="4:17" ht="30" customHeight="1">
+    <row r="10" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1204,7 +1443,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:17" ht="30" customHeight="1">
+    <row r="11" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1215,11 +1454,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:17" ht="30" customHeight="1"/>
-    <row r="13" spans="4:17" ht="30" customHeight="1"/>
-    <row r="14" spans="4:17" ht="30" customHeight="1"/>
-    <row r="15" spans="4:17" ht="30" customHeight="1"/>
-    <row r="16" spans="4:17" ht="30" customHeight="1"/>
+    <row r="12" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1231,29 +1470,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="4:17" ht="30" customHeight="1"/>
-    <row r="3" spans="4:17" ht="30" customHeight="1"/>
-    <row r="4" spans="4:17" ht="30" customHeight="1"/>
-    <row r="5" spans="4:17" ht="30" customHeight="1">
+    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="30" customHeight="1">
+    <row r="6" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>17</v>
       </c>
@@ -1266,7 +1505,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:17" ht="30" customHeight="1">
+    <row r="7" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1277,7 +1516,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="4:17" ht="30" customHeight="1">
+    <row r="8" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1289,7 +1528,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:17" ht="30" customHeight="1">
+    <row r="9" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1302,7 +1541,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="4:17" ht="30" customHeight="1">
+    <row r="10" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1313,7 +1552,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:17" ht="30" customHeight="1">
+    <row r="11" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1324,11 +1563,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:17" ht="30" customHeight="1"/>
-    <row r="13" spans="4:17" ht="30" customHeight="1"/>
-    <row r="14" spans="4:17" ht="30" customHeight="1"/>
-    <row r="15" spans="4:17" ht="30" customHeight="1"/>
-    <row r="16" spans="4:17" ht="30" customHeight="1"/>
+    <row r="12" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1340,29 +1579,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="4:17" ht="30" customHeight="1"/>
-    <row r="3" spans="4:17" ht="30" customHeight="1"/>
-    <row r="4" spans="4:17" ht="30" customHeight="1"/>
-    <row r="5" spans="4:17" ht="30" customHeight="1">
+    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="30" customHeight="1">
+    <row r="6" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>19</v>
       </c>
@@ -1375,7 +1614,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:17" ht="30" customHeight="1">
+    <row r="7" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1386,7 +1625,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="4:17" ht="30" customHeight="1">
+    <row r="8" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1398,7 +1637,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:17" ht="30" customHeight="1">
+    <row r="9" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1411,7 +1650,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="4:17" ht="30" customHeight="1">
+    <row r="10" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1422,7 +1661,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:17" ht="30" customHeight="1">
+    <row r="11" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1433,11 +1672,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:17" ht="30" customHeight="1"/>
-    <row r="13" spans="4:17" ht="30" customHeight="1"/>
-    <row r="14" spans="4:17" ht="30" customHeight="1"/>
-    <row r="15" spans="4:17" ht="30" customHeight="1"/>
-    <row r="16" spans="4:17" ht="30" customHeight="1"/>
+    <row r="12" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1449,29 +1688,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="4:17" ht="30" customHeight="1"/>
-    <row r="3" spans="4:17" ht="30" customHeight="1"/>
-    <row r="4" spans="4:17" ht="30" customHeight="1"/>
-    <row r="5" spans="4:17" ht="30" customHeight="1">
+    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="30" customHeight="1">
+    <row r="6" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>21</v>
       </c>
@@ -1484,7 +1723,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:17" ht="30" customHeight="1">
+    <row r="7" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1495,7 +1734,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="4:17" ht="30" customHeight="1">
+    <row r="8" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1507,7 +1746,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:17" ht="30" customHeight="1">
+    <row r="9" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1520,7 +1759,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="4:17" ht="30" customHeight="1">
+    <row r="10" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1531,7 +1770,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:17" ht="30" customHeight="1">
+    <row r="11" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1542,11 +1781,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:17" ht="30" customHeight="1"/>
-    <row r="13" spans="4:17" ht="30" customHeight="1"/>
-    <row r="14" spans="4:17" ht="30" customHeight="1"/>
-    <row r="15" spans="4:17" ht="30" customHeight="1"/>
-    <row r="16" spans="4:17" ht="30" customHeight="1"/>
+    <row r="12" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1558,29 +1797,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="4:17" ht="30" customHeight="1"/>
-    <row r="3" spans="4:17" ht="30" customHeight="1"/>
-    <row r="4" spans="4:17" ht="30" customHeight="1"/>
-    <row r="5" spans="4:17" ht="30" customHeight="1">
+    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="30" customHeight="1">
+    <row r="6" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1593,7 +1832,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:17" ht="30" customHeight="1">
+    <row r="7" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1604,7 +1843,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="4:17" ht="30" customHeight="1">
+    <row r="8" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1616,7 +1855,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:17" ht="30" customHeight="1">
+    <row r="9" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
@@ -1629,7 +1868,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="4:17" ht="30" customHeight="1">
+    <row r="10" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1640,7 +1879,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:17" ht="30" customHeight="1">
+    <row r="11" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1651,11 +1890,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:17" ht="30" customHeight="1"/>
-    <row r="13" spans="4:17" ht="30" customHeight="1"/>
-    <row r="14" spans="4:17" ht="30" customHeight="1"/>
-    <row r="15" spans="4:17" ht="30" customHeight="1"/>
-    <row r="16" spans="4:17" ht="30" customHeight="1"/>
+    <row r="12" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1667,29 +1906,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="4:17" ht="30" customHeight="1"/>
-    <row r="3" spans="4:17" ht="30" customHeight="1"/>
-    <row r="4" spans="4:17" ht="30" customHeight="1"/>
-    <row r="5" spans="4:17" ht="30" customHeight="1">
+    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="30" customHeight="1">
+    <row r="6" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1702,7 +1941,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:17" ht="30" customHeight="1">
+    <row r="7" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1713,7 +1952,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="4:17" ht="30" customHeight="1">
+    <row r="8" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1725,7 +1964,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:17" ht="30" customHeight="1">
+    <row r="9" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1738,7 +1977,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="4:17" ht="30" customHeight="1">
+    <row r="10" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1749,7 +1988,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:17" ht="30" customHeight="1">
+    <row r="11" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1760,11 +1999,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:17" ht="30" customHeight="1"/>
-    <row r="13" spans="4:17" ht="30" customHeight="1"/>
-    <row r="14" spans="4:17" ht="30" customHeight="1"/>
-    <row r="15" spans="4:17" ht="30" customHeight="1"/>
-    <row r="16" spans="4:17" ht="30" customHeight="1"/>
+    <row r="12" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1776,29 +2015,29 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="4:17" ht="30" customHeight="1"/>
-    <row r="3" spans="4:17" ht="30" customHeight="1"/>
-    <row r="4" spans="4:17" ht="30" customHeight="1"/>
-    <row r="5" spans="4:17" ht="30" customHeight="1">
+    <row r="1" spans="4:17" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="4:17" ht="30" customHeight="1">
+    <row r="6" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>0</v>
       </c>
@@ -1811,7 +2050,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="4:17" ht="30" customHeight="1">
+    <row r="7" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1822,7 +2061,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="4:17" ht="30" customHeight="1">
+    <row r="8" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1834,7 +2073,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="4:17" ht="30" customHeight="1">
+    <row r="9" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1847,7 +2086,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="4:17" ht="30" customHeight="1">
+    <row r="10" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1858,7 +2097,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="4:17" ht="30" customHeight="1">
+    <row r="11" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1869,11 +2108,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="4:17" ht="30" customHeight="1"/>
-    <row r="13" spans="4:17" ht="30" customHeight="1"/>
-    <row r="14" spans="4:17" ht="30" customHeight="1"/>
-    <row r="15" spans="4:17" ht="30" customHeight="1"/>
-    <row r="16" spans="4:17" ht="30" customHeight="1"/>
+    <row r="12" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>
@@ -1885,25 +2124,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1"/>
-    <row r="2" spans="6:14" ht="30" customHeight="1"/>
-    <row r="3" spans="6:14" ht="30" customHeight="1"/>
-    <row r="4" spans="6:14" ht="30" customHeight="1"/>
-    <row r="5" spans="6:14" ht="30" customHeight="1"/>
-    <row r="6" spans="6:14" ht="30" customHeight="1">
+    <row r="1" spans="6:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1916,7 +2155,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="6:14" ht="30" customHeight="1">
+    <row r="7" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1927,7 +2166,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="6:14" ht="30" customHeight="1">
+    <row r="8" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1938,7 +2177,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="6:14" ht="30" customHeight="1">
+    <row r="9" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1951,7 +2190,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="6:14" ht="30" customHeight="1">
+    <row r="10" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1962,7 +2201,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="6:14" ht="30" customHeight="1">
+    <row r="11" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1973,11 +2212,11 @@
       <c r="M11" s="5"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="6:14" ht="30" customHeight="1"/>
-    <row r="13" spans="6:14" ht="30" customHeight="1"/>
-    <row r="14" spans="6:14" ht="30" customHeight="1"/>
-    <row r="15" spans="6:14" ht="30" customHeight="1"/>
-    <row r="16" spans="6:14" ht="30" customHeight="1"/>
+    <row r="12" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="6:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:M8"/>

</xml_diff>